<commit_message>
Altera doc de analise de concorrencia
</commit_message>
<xml_diff>
--- a/Documentos/Análise de concorrência/Análise de concorrência.xlsx
+++ b/Documentos/Análise de concorrência/Análise de concorrência.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victor.pederzini\Documents\miaudote\Documentos\Análise de concorrência\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isabella.silva\Desktop\Bandtec\4 semestre\miaudote\Documentos\Análise de concorrência\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77CB618-F43E-4551-9B6F-CF9A2F58F2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D52C1A-F5D8-43C2-AD0A-07E231265C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40700360-EB9B-42F8-AF56-2F27CD13BB1C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{40700360-EB9B-42F8-AF56-2F27CD13BB1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Victor" sheetId="1" r:id="rId1"/>
+    <sheet name="Isabella" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Funcionalidade</t>
   </si>
@@ -82,6 +83,21 @@
   </si>
   <si>
     <t>AdotaPet</t>
+  </si>
+  <si>
+    <t>Hyppet</t>
+  </si>
+  <si>
+    <t>PETTS</t>
+  </si>
+  <si>
+    <t>Adopt me</t>
+  </si>
+  <si>
+    <t>Pet Finder</t>
+  </si>
+  <si>
+    <t>AdotaFácil</t>
   </si>
 </sst>
 </file>
@@ -3318,8 +3334,2913 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>415176</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>25945</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>639576</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>285745</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Graphic 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6077AFC3-EEDD-40D3-B055-E7CEC0EB7B62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3720351" y="816520"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>396126</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>53378</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>620526</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>313178</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Graphic 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F0C528A-705B-4172-821D-9317AAFE9FF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3701301" y="1167803"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>377076</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>33187</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>601476</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>292987</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Graphic 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D961A318-5297-4EDC-9B59-A9A3B504EC9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3682251" y="1480987"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>367551</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>59479</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>591951</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>319279</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Graphic 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C9B4CA2-710C-4C32-B43C-FEA87DE9E0FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3672726" y="2174029"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>377076</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38145</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>601476</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>297945</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Graphic 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4754193-C408-4FDF-BE45-0DB71DB918D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3682251" y="2848020"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>377076</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>37004</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>601476</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>296804</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Graphic 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF68B967-9D82-4DC1-9B2D-ED3259C5E5E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3682251" y="3189779"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>387302</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>64433</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>572201</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>306482</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Graphic 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44371308-BA88-4F70-AAEC-3D5AD8CE0675}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3692477" y="3522008"/>
+          <a:ext cx="184899" cy="242049"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>375859</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>27084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>600259</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>286884</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Graphic 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A1C56E6-228A-4BFA-A166-6751957B2AB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4185859" y="1979709"/>
+          <a:ext cx="224400" cy="183600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>404434</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>21631</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>628834</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>281431</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Graphic 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4B09595-BF82-421A-9D47-821BCA4C4FC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4833559" y="1136056"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>395610</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>27821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>580509</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>288920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Graphic 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2D0F2C8-65F3-439A-B8DB-9A4BDD18C451}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4205610" y="1447046"/>
+          <a:ext cx="184899" cy="184899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>375859</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>29489</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>600259</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>289289</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Graphic 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3835F96C-C92A-4A1F-A67E-AFF814B479DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4185859" y="1220114"/>
+          <a:ext cx="224400" cy="183600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>442534</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>33192</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>666934</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>292992</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Graphic 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08C9CB88-0A28-4F7F-BD35-1407AAB3FF5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4871659" y="499917"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>375859</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>25048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>600259</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>284848</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Graphic 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0E12706-4A18-4514-9FDC-51506E5B330D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4185859" y="2472973"/>
+          <a:ext cx="224400" cy="183600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>431834</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>56222</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>616733</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>298271</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Graphic 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7D08BA0-7D8F-4AE7-B4F2-C79F9A85F581}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5889659" y="3208997"/>
+          <a:ext cx="184899" cy="242049"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>460409</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>70865</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>645308</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>8114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Graphic 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A00FFFC0-8589-4440-8E9A-1BD28479AFB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5918234" y="1861565"/>
+          <a:ext cx="184899" cy="261099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>441359</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>58269</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>626258</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>319368</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Graphic 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{588D1970-CA97-447B-8493-F54D37BDE6A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5899184" y="2525244"/>
+          <a:ext cx="184899" cy="261099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>441359</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>626258</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Graphic 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C676FE6-8377-4C90-84C2-AE96E0DC52BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5899184" y="2895696"/>
+          <a:ext cx="184899" cy="261099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>391392</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>50174</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>615792</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>300449</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Graphic 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B14AFAA7-48B5-47AF-8F21-9484E661122A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5858742" y="1240799"/>
+          <a:ext cx="224400" cy="174075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>411143</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>47994</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>596042</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>309093</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Graphic 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7963C4B5-D844-445F-AFBC-BAEA2698D29A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5878493" y="1467219"/>
+          <a:ext cx="184899" cy="184899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>391392</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>46233</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>615792</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>306033</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Graphic 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4DFC792-1939-4388-8615-B64D17C4EFBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5858742" y="1998858"/>
+          <a:ext cx="224400" cy="183600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>411143</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>44053</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>596042</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>305152</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Graphic 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BD3AB1F-D3EB-459A-8DE3-666987D6A910}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5878493" y="2263378"/>
+          <a:ext cx="184899" cy="184899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>411143</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>54114</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>596042</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>305688</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Graphic 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CBFE3E9-A2E5-4DC2-A53A-DEE93943092D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5878493" y="520839"/>
+          <a:ext cx="184899" cy="175374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>411143</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>42291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>596042</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>284340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Graphic 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A7EB1EE-8D81-4072-86B2-44FF810F1A5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5878493" y="2718816"/>
+          <a:ext cx="184899" cy="184899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457081</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>37867</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>681481</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>297667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Graphic 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CA7F9FC-8D40-4D60-9092-EA75512B5A97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8181856" y="2504842"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457782</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>36465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>642681</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>297564</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Graphic 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD95A83D-1D44-42F1-8D8E-1A2DEA4A360E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8182557" y="2846340"/>
+          <a:ext cx="184899" cy="261099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438031</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>26838</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>662431</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>286638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Graphic 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{199A3813-3060-4288-A777-EE7C4A7A5130}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8162806" y="3179613"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>410157</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>63536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>595056</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>305585</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Graphic 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A68CA3A-D6A4-42F4-A45E-DE8AD3E6AED8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8134932" y="3521111"/>
+          <a:ext cx="184899" cy="242049"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>476131</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>50298</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>700531</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>300573</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Graphic 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BF215D5-80A4-43EF-8D87-8060515414FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8200906" y="1498098"/>
+          <a:ext cx="224400" cy="250275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>173173</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2200275</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Imagem 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AC9793C-6747-4921-AC86-14AF17F69B82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619125" y="3945073"/>
+          <a:ext cx="2190750" cy="4808402"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2314576</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>655321</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Imagem 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{852FE2EE-639F-4A8D-BB07-59B6DA24BD8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2924176" y="3962401"/>
+          <a:ext cx="2160270" cy="4800600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Imagem 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C080E68-9C30-45CB-A3CA-84B99EE93E40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5133975" y="3962400"/>
+          <a:ext cx="2162175" cy="4804833"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2382</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Imagem 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D71CC73E-A598-44C4-8A34-F1344D2FEBF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7467600" y="3962400"/>
+          <a:ext cx="2164557" cy="4810125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Imagem 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70B52DD3-22F0-43DC-AED2-2E89448453DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9734550" y="3962400"/>
+          <a:ext cx="2162175" cy="4804833"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>450884</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76258</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>635783</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>13507</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="Graphic 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBF317A6-2C6B-4639-AEEF-21B17FF5A000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3756059" y="542983"/>
+          <a:ext cx="184899" cy="261099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>405135</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>65921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590034</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3170</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="63" name="Graphic 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76E3E046-D0F4-4673-A411-5333C9BEE08B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3710310" y="1856621"/>
+          <a:ext cx="184899" cy="261099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>395610</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>46871</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>580509</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>307970</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Graphic 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F12F2BB0-818C-469C-A4A7-0155A1ED8770}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3700785" y="2513846"/>
+          <a:ext cx="184899" cy="261099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>423484</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>33192</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>647884</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>292992</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="65" name="Graphic 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E47C395A-D864-47D3-BE27-F4754EFECB7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4852609" y="823767"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>366334</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>48539</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590734</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>308339</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="Graphic 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE97907-C0BC-4262-8E80-A5632253A551}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4795459" y="2163089"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>366334</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>36609</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590734</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>296409</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="67" name="Graphic 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93920D0D-EB75-4995-8B14-F59B7A067439}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4795459" y="2846484"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>393734</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>65747</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>578633</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>307796</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="Graphic 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F33E213-0387-4479-A61F-9E8E16D29B7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4822859" y="3523322"/>
+          <a:ext cx="184899" cy="242049"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>479459</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>51815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>664358</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>312914</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="Graphic 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EBAB381-8193-4422-8815-08E5060376AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5937284" y="518540"/>
+          <a:ext cx="184899" cy="261099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>442534</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>52242</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>666934</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>312042</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="73" name="Graphic 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18FCC19A-56FB-44CE-BF63-16C90E8F60C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5900359" y="842817"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>469934</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>80390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>654833</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>8114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="Graphic 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{794EE1B7-87D7-4383-B76C-05C170C14CB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5927759" y="1194815"/>
+          <a:ext cx="184899" cy="261099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>433009</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>52242</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>657409</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>312042</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="75" name="Graphic 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1284A87F-CA1C-4068-B44C-01837ED2741B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5890834" y="1500042"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>433009</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>42717</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>657409</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>302517</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="76" name="Graphic 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBAF9104-0943-4B08-9F48-BC0B1B9828DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5890834" y="2157267"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>431834</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>65747</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>616733</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>307796</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="77" name="Graphic 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56CF8FC6-1926-49A6-9CA5-10C3A8F53BE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5889659" y="3523322"/>
+          <a:ext cx="184899" cy="242049"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>400917</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>17658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>625317</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>277458</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="78" name="Graphic 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C872A07-D2FB-40E3-917D-07E3FB44D54A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7001742" y="3170433"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381867</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>33303</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>606267</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>293103</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="79" name="Graphic 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{360D398A-76E9-4686-807C-5AAF0C40ACC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6982692" y="823878"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>400632</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>78975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>585531</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>6699</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="80" name="Graphic 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB271721-3A61-4D24-84BF-49EABC4A46C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7001457" y="1193400"/>
+          <a:ext cx="184899" cy="261099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>399931</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>48896</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>624331</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>308696</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="81" name="Graphic 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC356A8B-900B-4E59-989D-CDBD50D013FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7000756" y="2163446"/>
+          <a:ext cx="224400" cy="259800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>466606</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>21723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>691006</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>271998</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="82" name="Graphic 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1DC3CE0-39E1-4493-803E-FE9FB8DD9A85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8191381" y="812298"/>
+          <a:ext cx="224400" cy="250275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457081</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>31248</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>681481</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>281523</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="83" name="Graphic 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{143B5DF2-50C4-43E7-BDEB-3D3ECFE939D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8181856" y="497973"/>
+          <a:ext cx="224400" cy="250275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>466606</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>59823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>691006</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>310098</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="84" name="Graphic 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D3AC939-014B-457F-94BA-35A3E539F8C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8191381" y="1174248"/>
+          <a:ext cx="224400" cy="250275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>486357</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>47495</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>671256</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>308594</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="85" name="Graphic 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{459F9D55-8C1C-4990-824F-522EBACBD9A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8211132" y="1838195"/>
+          <a:ext cx="184899" cy="261099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438031</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>40773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>662431</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>291048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="86" name="Graphic 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7518CEA7-D85F-47F2-AC14-3DE66FBCE0B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8162806" y="2155323"/>
+          <a:ext cx="224400" cy="250275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3617,8 +6538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9731F11E-6F62-4021-8440-72F7CDD679E9}">
   <dimension ref="B1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3652,7 +6573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
@@ -3662,7 +6583,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="2:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
@@ -3682,7 +6603,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="2:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>4</v>
       </c>
@@ -3722,7 +6643,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="2:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -3732,7 +6653,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="2:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
@@ -3784,4 +6705,149 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0725C0-22C1-4010-A486-68A0A37EC40E}">
+  <dimension ref="B1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="2:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="2:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>